<commit_message>
Se agregaron los S.O.Pln correspondientes y se generalizo el Beta y el Alpha
</commit_message>
<xml_diff>
--- a/Matrices/TiempoDeLasTransiciones.xlsx
+++ b/Matrices/TiempoDeLasTransiciones.xlsx
@@ -10,10 +10,10 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -24,11 +24,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+  <fonts count="4">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -46,14 +45,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,7 +94,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,88 +118,83 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:T1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>30000</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>24000</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="n">
+        <v>30000000000</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>24000000000</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>5000</v>
+        <v>500000000</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>15000</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>18000</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>21000</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T1" s="1" t="n">
+        <v>15000000000</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>18000000000</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>10000000000</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P1" s="0" t="n">
+        <v>21000000000</v>
+      </c>
+      <c r="Q1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T1" s="0" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>